<commit_message>
Changes to Downsizer scripts
</commit_message>
<xml_diff>
--- a/Documentation/StationList.xlsx
+++ b/Documentation/StationList.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palemi\Documents\Github\DWRAT_DataScraping\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE29F99C-7D1B-4F35-9386-95E2A043A025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD092A0-EEA5-493B-998D-4180665A97FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="10785" xr2:uid="{0EE69560-0D0F-42D9-B69C-8F6D2FF31780}"/>
+    <workbookView xWindow="-21195" yWindow="3630" windowWidth="21585" windowHeight="11505" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
   </bookViews>
   <sheets>
     <sheet name="StationList" sheetId="1" r:id="rId1"/>
-    <sheet name="DownloadGuide" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="DownloadGuide" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="107">
   <si>
     <t>Source</t>
   </si>
@@ -246,9 +246,6 @@
     <t>SKPC1</t>
   </si>
   <si>
-    <t>Downsizer</t>
-  </si>
-  <si>
     <t>TMIN1</t>
   </si>
   <si>
@@ -310,6 +307,96 @@
   </si>
   <si>
     <t>PRECIP4</t>
+  </si>
+  <si>
+    <t>1  049684precip39.4194-123.34251353</t>
+  </si>
+  <si>
+    <t>2  047109precip39.3619-123.12861018</t>
+  </si>
+  <si>
+    <t>3   049122precip39.1466-123.2102636</t>
+  </si>
+  <si>
+    <t>4  049126precip39.1266-123.27191328</t>
+  </si>
+  <si>
+    <t>5    041838precip38.793-123.0263400</t>
+  </si>
+  <si>
+    <t>6   043875precip38.6294-122.8665177</t>
+  </si>
+  <si>
+    <t>7   041312precip38.5768-122.5781350</t>
+  </si>
+  <si>
+    <t>8    043191precip38.515-123.2447112</t>
+  </si>
+  <si>
+    <t>9   043578precip38.4305-122.8647200</t>
+  </si>
+  <si>
+    <t>10  046370precip38.3858-122.9661865</t>
+  </si>
+  <si>
+    <t>11   049684tmax39.4194-123.34251353</t>
+  </si>
+  <si>
+    <t>12   047109tmax39.3619-123.12861018</t>
+  </si>
+  <si>
+    <t>13    049122tmax39.1466-123.2102636</t>
+  </si>
+  <si>
+    <t>14   049126tmax39.1266-123.27191328</t>
+  </si>
+  <si>
+    <t>15     041838tmax38.793-123.0263400</t>
+  </si>
+  <si>
+    <t>16    043875tmax38.6294-122.8665177</t>
+  </si>
+  <si>
+    <t>17    041312tmax38.5768-122.5781350</t>
+  </si>
+  <si>
+    <t>18     043191tmax38.515-123.2447112</t>
+  </si>
+  <si>
+    <t>19    043578tmax38.4305-122.8647200</t>
+  </si>
+  <si>
+    <t>20    046370tmax38.3858-122.9661865</t>
+  </si>
+  <si>
+    <t>21   049684tmin39.4194-123.34251353</t>
+  </si>
+  <si>
+    <t>22   047109tmin39.3619-123.12861018</t>
+  </si>
+  <si>
+    <t>23    049122tmin39.1466-123.2102636</t>
+  </si>
+  <si>
+    <t>24   049126tmin39.1266-123.27191328</t>
+  </si>
+  <si>
+    <t>25     041838tmin38.793-123.0263400</t>
+  </si>
+  <si>
+    <t>26    043875tmin38.6294-122.8665177</t>
+  </si>
+  <si>
+    <t>27    041312tmin38.5768-122.5781350</t>
+  </si>
+  <si>
+    <t>28     043191tmin38.515-123.2447112</t>
+  </si>
+  <si>
+    <t>29    043578tmin38.4305-122.8647200</t>
+  </si>
+  <si>
+    <t>30    046370tmin38.3858-122.9661865</t>
   </si>
 </sst>
 </file>
@@ -805,10 +892,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1712,12 +1799,12 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="CIMIS" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
-  <location ref="D3:D11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="D3:D29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="5">
-        <item x="2"/>
-        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item x="0"/>
         <item h="1" x="3"/>
         <item h="1" x="1"/>
         <item t="default"/>
@@ -1788,30 +1875,84 @@
     <field x="3"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="26">
     <i>
-      <x v="24"/>
+      <x/>
     </i>
     <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i>
       <x v="7"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
     <i>
-      <x v="33"/>
+      <x v="8"/>
     </i>
     <i r="1">
-      <x v="2"/>
+      <x v="1"/>
     </i>
     <i>
-      <x v="35"/>
+      <x v="9"/>
     </i>
     <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
+      <x v="1"/>
     </i>
   </rowItems>
   <colItems count="1">
@@ -2110,7 +2251,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:H64" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A2:H64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A2:H64" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="DOWNSIZER"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H64">
     <sortCondition ref="B2:B64" customList="PRECIP1,PRECIP2,PRECIP3,PRECIP4,PRECIP5,PRECIP6,PRECIP7,PRECIP8,PRECIP9,PRECIP10,PRECIP11,PRECIP12,PRECIP13,PRECIP14,PRECIP15,TMAX1,TMIN1,TMAX2,TMIN2,TMAX3,TMIN3,TMAX4,TMIN4,TMAX5,TMIN5,TMAX6,TMIN6,TMAX7,TMIN8,TMAX8,TMIN8"/>
   </sortState>
@@ -2417,7 +2564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2444,12 +2591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="C32" sqref="C4:C32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2463,8 +2605,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>75</v>
+      <c r="A1" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2493,15 +2635,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2">
         <v>49684</v>
@@ -2571,15 +2713,15 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2">
         <v>47109</v>
@@ -2623,15 +2765,15 @@
         <v>636</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2">
         <v>49122</v>
@@ -2649,26 +2791,26 @@
         <v>6369</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -2706,15 +2848,15 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2">
         <v>49126</v>
@@ -2732,12 +2874,12 @@
         <v>132811</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -2749,21 +2891,21 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2780,15 +2922,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -2820,15 +2962,15 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2">
         <v>41838</v>
@@ -2846,7 +2988,7 @@
         <v>40014</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2863,29 +3005,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="2">
         <v>43875</v>
@@ -2929,15 +3071,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" s="2">
         <v>41312</v>
@@ -2981,21 +3123,21 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -3012,15 +3154,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="2">
         <v>43191</v>
@@ -3064,15 +3206,15 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="2">
         <v>43578</v>
@@ -3116,15 +3258,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="2">
         <v>46370</v>
@@ -3194,15 +3336,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="2">
         <v>43875</v>
@@ -3210,10 +3352,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
         <v>56</v>
-      </c>
-      <c r="B35" t="s">
-        <v>57</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
@@ -3222,7 +3364,7 @@
         <v>43875</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F35">
         <v>38.629399999999997</v>
@@ -3234,29 +3376,29 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="2">
         <v>43875</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="2">
         <v>49122</v>
@@ -3290,10 +3432,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
@@ -3302,7 +3444,7 @@
         <v>49122</v>
       </c>
       <c r="E39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F39">
         <v>39.146599999999999</v>
@@ -3314,35 +3456,35 @@
         <v>636</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" s="2">
         <v>49122</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
         <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -3359,12 +3501,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
         <v>28</v>
@@ -3376,35 +3518,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
         <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -3421,12 +3563,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
         <v>41</v>
@@ -3438,35 +3580,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
         <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3483,7 +3625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3500,29 +3642,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D53" s="2">
         <v>47109</v>
@@ -3556,10 +3698,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
@@ -3568,7 +3710,7 @@
         <v>47109</v>
       </c>
       <c r="E55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F55">
         <v>39.361899999999999</v>
@@ -3580,35 +3722,35 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D56" s="2">
         <v>47109</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B57" t="s">
         <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3625,88 +3767,88 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E59" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>67</v>
       </c>
-      <c r="C60" t="s">
-        <v>74</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>68</v>
-      </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
       <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
         <v>64</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E62" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64" t="s">
         <v>55</v>
@@ -3719,7 +3861,7 @@
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
+      <c r="A66" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3732,13 +3874,178 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2A0C3C-9CB2-4C3C-9D1B-CDB48F934EC5}">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:H7"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3747,8 +4054,8 @@
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -3808,21 +4115,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3841,7 +4148,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>28</v>
@@ -3852,10 +4159,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>70</v>
+      </c>
+      <c r="D4" s="1">
+        <v>41312</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>39</v>
@@ -3868,8 +4175,8 @@
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4">
-        <v>-999</v>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
@@ -3882,8 +4189,8 @@
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>37</v>
+      <c r="D6" s="1">
+        <v>41838</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>17</v>
@@ -3897,7 +4204,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
@@ -3910,8 +4217,8 @@
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
+      <c r="D8" s="1">
+        <v>43191</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>13</v>
@@ -3925,7 +4232,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>41</v>
@@ -3938,8 +4245,8 @@
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>50</v>
+      <c r="D10" s="1">
+        <v>43578</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>36</v>
@@ -3950,10 +4257,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>34</v>
@@ -3966,6 +4273,9 @@
       <c r="A12" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="D12" s="1">
+        <v>43875</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>55</v>
       </c>
@@ -3974,14 +4284,20 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
       </c>
@@ -3990,11 +4306,84 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="G15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H15">
         <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>46370</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>47109</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <v>49122</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <v>49126</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
+        <v>49684</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -4007,15 +4396,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F312EB754F236045A0D3EDD082CC91AE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="241ce865d663be13d7e342f59527821d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06" xmlns:ns3="851dfaa3-aae8-4c03-b90c-7dd4a6526d0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3129014a3b2306d1c4ed4239399361fd" ns2:_="" ns3:_="">
     <xsd:import namespace="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06"/>
@@ -4192,15 +4572,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2643DE3-C6DD-4C5A-9AE4-EF5AECAB0779}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4217,4 +4598,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating CIMIS_Scraper.R to export all processed CIMIS data in 1 CSV, CIMIS_Processed.csv
</commit_message>
<xml_diff>
--- a/Documentation/StationList.xlsx
+++ b/Documentation/StationList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palemi\Documents\Github\DWRAT_DataScraping\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD092A0-EEA5-493B-998D-4180665A97FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9ECA16-BE6B-44AA-810A-6E016771F8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21195" yWindow="3630" windowWidth="21585" windowHeight="11505" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
+    <workbookView xWindow="885" yWindow="2085" windowWidth="21585" windowHeight="11505" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
   </bookViews>
   <sheets>
     <sheet name="StationList" sheetId="1" r:id="rId1"/>
@@ -2251,13 +2251,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:H64" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A2:H64" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="DOWNSIZER"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:H64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H64">
     <sortCondition ref="B2:B64" customList="PRECIP1,PRECIP2,PRECIP3,PRECIP4,PRECIP5,PRECIP6,PRECIP7,PRECIP8,PRECIP9,PRECIP10,PRECIP11,PRECIP12,PRECIP13,PRECIP14,PRECIP15,TMAX1,TMIN1,TMAX2,TMIN2,TMAX3,TMIN3,TMAX4,TMIN4,TMAX5,TMIN5,TMAX6,TMIN6,TMAX7,TMIN8,TMAX8,TMIN8"/>
   </sortState>
@@ -2591,7 +2585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2635,7 +2631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2713,7 +2709,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2765,7 +2761,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2791,7 +2787,7 @@
         <v>6369</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -2805,7 +2801,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2848,7 +2844,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2874,7 +2870,7 @@
         <v>132811</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2891,7 +2887,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2905,7 +2901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2922,7 +2918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2962,7 +2958,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -2988,7 +2984,7 @@
         <v>40014</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -3005,7 +3001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -3019,7 +3015,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -3071,7 +3067,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3123,7 +3119,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3137,7 +3133,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -3154,7 +3150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3206,7 +3202,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -3258,7 +3254,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -3336,7 +3332,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -3376,7 +3372,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -3390,7 +3386,7 @@
         <v>43875</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -3456,7 +3452,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3470,7 +3466,7 @@
         <v>49122</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -3484,7 +3480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -3501,7 +3497,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -3518,7 +3514,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -3532,7 +3528,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -3546,7 +3542,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -3563,7 +3559,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -3580,7 +3576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -3594,7 +3590,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -3608,7 +3604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3625,7 +3621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3642,7 +3638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -3656,7 +3652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -3722,7 +3718,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -3736,7 +3732,7 @@
         <v>47109</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3750,7 +3746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3767,7 +3763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3784,7 +3780,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -3798,7 +3794,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3812,7 +3808,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -3829,7 +3825,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -3843,7 +3839,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -4396,6 +4392,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F312EB754F236045A0D3EDD082CC91AE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="241ce865d663be13d7e342f59527821d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06" xmlns:ns3="851dfaa3-aae8-4c03-b90c-7dd4a6526d0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3129014a3b2306d1c4ed4239399361fd" ns2:_="" ns3:_="">
     <xsd:import namespace="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06"/>
@@ -4572,16 +4577,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2643DE3-C6DD-4C5A-9AE4-EF5AECAB0779}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4598,12 +4602,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Wrote Dat_Shell_Generation.R and deleted DAT_File_Manipulation.R
</commit_message>
<xml_diff>
--- a/Documentation/StationList.xlsx
+++ b/Documentation/StationList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palemi\Documents\Github\DWRAT_DataScraping\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9ECA16-BE6B-44AA-810A-6E016771F8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F017DE3-B2E9-4B00-9A0B-6C9F776B2EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="2085" windowWidth="21585" windowHeight="11505" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
+    <workbookView xWindow="-26160" yWindow="2430" windowWidth="21585" windowHeight="11505" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
   </bookViews>
   <sheets>
     <sheet name="StationList" sheetId="1" r:id="rId1"/>
@@ -2251,7 +2251,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:H64" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A2:H64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A2:H64" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="DOWNSIZER"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H64">
     <sortCondition ref="B2:B64" customList="PRECIP1,PRECIP2,PRECIP3,PRECIP4,PRECIP5,PRECIP6,PRECIP7,PRECIP8,PRECIP9,PRECIP10,PRECIP11,PRECIP12,PRECIP13,PRECIP14,PRECIP15,TMAX1,TMIN1,TMAX2,TMIN2,TMAX3,TMIN3,TMAX4,TMIN4,TMAX5,TMIN5,TMAX6,TMIN6,TMAX7,TMIN8,TMAX8,TMIN8"/>
   </sortState>
@@ -2586,7 +2592,7 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2631,7 +2637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2761,7 +2767,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2787,7 +2793,7 @@
         <v>6369</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2844,7 +2850,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>132811</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2887,7 +2893,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2918,7 +2924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2958,7 +2964,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>40014</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -3015,7 +3021,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3119,7 +3125,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3133,7 +3139,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -3150,7 +3156,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3202,7 +3208,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -3254,7 +3260,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -3332,7 +3338,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -3386,7 +3392,7 @@
         <v>43875</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -3452,7 +3458,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3466,7 +3472,7 @@
         <v>49122</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -3480,7 +3486,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -3497,7 +3503,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -3514,7 +3520,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -3528,7 +3534,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -3542,7 +3548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -3559,7 +3565,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -3576,7 +3582,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -3590,7 +3596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3621,7 +3627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3638,7 +3644,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -3652,7 +3658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -3718,7 +3724,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -3732,7 +3738,7 @@
         <v>47109</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3746,7 +3752,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3763,7 +3769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -3794,7 +3800,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3808,7 +3814,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -3839,7 +3845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -4392,15 +4398,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F312EB754F236045A0D3EDD082CC91AE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="241ce865d663be13d7e342f59527821d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06" xmlns:ns3="851dfaa3-aae8-4c03-b90c-7dd4a6526d0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3129014a3b2306d1c4ed4239399361fd" ns2:_="" ns3:_="">
     <xsd:import namespace="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06"/>
@@ -4577,15 +4574,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2643DE3-C6DD-4C5A-9AE4-EF5AECAB0779}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4602,4 +4600,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>